<commit_message>
scraper for IMDb Failed because of GFW.
</commit_message>
<xml_diff>
--- a/rst/ExamRst.xlsx
+++ b/rst/ExamRst.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="26895" windowHeight="12960" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="26895" windowHeight="12960" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="MAP" sheetId="1" r:id="rId1"/>
     <sheet name="LatentDimensions" sheetId="2" r:id="rId2"/>
     <sheet name="Recall@N" sheetId="3" r:id="rId3"/>
     <sheet name="CDL" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>CL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +97,93 @@
   </si>
   <si>
     <t>MAP@10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>数据量（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>耗时（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>Out of memory</t>
+  </si>
+  <si>
+    <r>
+      <t>耗时（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>2 workers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 workers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 workers</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -103,7 +191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +214,32 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -135,12 +249,116 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -153,18 +371,42 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -174,6 +416,386 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>137.81100000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>216.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>236.49199999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>301.60899999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>307.35300000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350.38799999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>311.97000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>299.83600000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>366.94799999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>371.791</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>544.399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>788.77800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>993.048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1133.097</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1391.537</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1564.385</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1739.7149999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1983.9169999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2242.5030000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>318.22399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245.697</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205.596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243.59299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>308.63099999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>334.35300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>332.47399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>346.404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>374.13600000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350.18900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>503.33800000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>624.38400000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>725.59699999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>844.625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>972.55799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1111.2940000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1315.67</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1386.5940000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1524.6469999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>278.95699999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>242.654</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>287.88400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>325.58100000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>352.774</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>372.16300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>330.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>341.61700000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>355.37599999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>302.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>432.06400000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>559.83699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>651.03099999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>786.16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>896.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>959.03</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1068.357</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1175.758</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1271.675</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="84773888"/>
+        <c:axId val="84783872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="84773888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84783872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84783872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84773888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,7 +1109,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -507,7 +1129,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>0.2</v>
       </c>
@@ -525,7 +1147,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -543,7 +1165,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5">
         <v>0.6</v>
       </c>
@@ -561,7 +1183,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6">
         <v>0.8</v>
       </c>
@@ -579,7 +1201,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -597,7 +1219,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8">
@@ -617,7 +1239,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9">
         <v>0.2</v>
       </c>
@@ -635,7 +1257,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10">
         <v>0.4</v>
       </c>
@@ -653,7 +1275,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11">
         <v>0.6</v>
       </c>
@@ -671,7 +1293,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12">
         <v>0.8</v>
       </c>
@@ -689,7 +1311,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13">
         <v>1</v>
       </c>
@@ -707,7 +1329,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B14">
@@ -727,7 +1349,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15">
         <v>0.2</v>
       </c>
@@ -745,7 +1367,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16">
         <v>0.4</v>
       </c>
@@ -763,7 +1385,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17">
         <v>0.6</v>
       </c>
@@ -781,7 +1403,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18">
         <v>0.8</v>
       </c>
@@ -799,7 +1421,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -838,18 +1460,18 @@
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -866,7 +1488,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>20</v>
       </c>
@@ -881,7 +1503,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4">
         <v>50</v>
       </c>
@@ -896,7 +1518,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5">
         <v>100</v>
       </c>
@@ -911,7 +1533,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6">
@@ -919,25 +1541,25 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B10">
@@ -945,19 +1567,19 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13">
         <v>100</v>
       </c>
@@ -982,7 +1604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13:I14"/>
     </sheetView>
   </sheetViews>
@@ -1094,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1112,7 +1734,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B2">
@@ -1129,7 +1751,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>100</v>
       </c>
@@ -1144,7 +1766,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4">
         <v>150</v>
       </c>
@@ -1159,7 +1781,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5">
         <v>200</v>
       </c>
@@ -1174,7 +1796,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6">
         <v>250</v>
       </c>
@@ -1189,7 +1811,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7">
         <v>300</v>
       </c>
@@ -1204,7 +1826,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8">
@@ -1221,7 +1843,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9">
         <v>100</v>
       </c>
@@ -1236,7 +1858,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10">
         <v>150</v>
       </c>
@@ -1251,7 +1873,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11">
         <v>200</v>
       </c>
@@ -1266,7 +1888,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12">
         <v>250</v>
       </c>
@@ -1281,7 +1903,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13">
         <v>300</v>
       </c>
@@ -1307,7 +1929,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -1324,7 +1946,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
       <c r="B20">
         <v>100</v>
       </c>
@@ -1339,7 +1961,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21">
         <v>150</v>
       </c>
@@ -1354,7 +1976,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22">
         <v>200</v>
       </c>
@@ -1369,7 +1991,7 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23">
         <v>250</v>
       </c>
@@ -1384,7 +2006,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24">
         <v>300</v>
       </c>
@@ -1399,7 +2021,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25">
@@ -1416,7 +2038,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
       <c r="B26">
         <v>100</v>
       </c>
@@ -1431,7 +2053,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="2"/>
+      <c r="A27" s="3"/>
       <c r="B27">
         <v>150</v>
       </c>
@@ -1446,7 +2068,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
       <c r="B28">
         <v>200</v>
       </c>
@@ -1461,7 +2083,7 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="2"/>
+      <c r="A29" s="3"/>
       <c r="B29">
         <v>250</v>
       </c>
@@ -1476,7 +2098,7 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2"/>
+      <c r="A30" s="3"/>
       <c r="B30">
         <v>300</v>
       </c>
@@ -1500,4 +2122,355 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.89</v>
+      </c>
+      <c r="D2" s="10">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11">
+        <v>137.81100000000001</v>
+      </c>
+      <c r="F2" s="11">
+        <v>318.22399999999999</v>
+      </c>
+      <c r="G2" s="11">
+        <v>278.95699999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="D3" s="10">
+        <v>12</v>
+      </c>
+      <c r="E3" s="11">
+        <v>216.43</v>
+      </c>
+      <c r="F3" s="11">
+        <v>245.697</v>
+      </c>
+      <c r="G3" s="11">
+        <v>242.654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>59.8</v>
+      </c>
+      <c r="D4" s="10">
+        <v>18</v>
+      </c>
+      <c r="E4" s="11">
+        <v>236.49199999999999</v>
+      </c>
+      <c r="F4" s="11">
+        <v>205.596</v>
+      </c>
+      <c r="G4" s="11">
+        <v>287.88400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>146</v>
+      </c>
+      <c r="D5" s="10">
+        <v>24</v>
+      </c>
+      <c r="E5" s="11">
+        <v>301.60899999999998</v>
+      </c>
+      <c r="F5" s="11">
+        <v>243.59299999999999</v>
+      </c>
+      <c r="G5" s="11">
+        <v>325.58100000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>244</v>
+      </c>
+      <c r="D6" s="10">
+        <v>30</v>
+      </c>
+      <c r="E6" s="11">
+        <v>307.35300000000001</v>
+      </c>
+      <c r="F6" s="11">
+        <v>308.63099999999997</v>
+      </c>
+      <c r="G6" s="11">
+        <v>352.774</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>408</v>
+      </c>
+      <c r="D7" s="10">
+        <v>36</v>
+      </c>
+      <c r="E7" s="11">
+        <v>350.38799999999998</v>
+      </c>
+      <c r="F7" s="11">
+        <v>334.35300000000001</v>
+      </c>
+      <c r="G7" s="11">
+        <v>372.16300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1865</v>
+      </c>
+      <c r="D8" s="10">
+        <v>42</v>
+      </c>
+      <c r="E8" s="11">
+        <v>311.97000000000003</v>
+      </c>
+      <c r="F8" s="11">
+        <v>332.47399999999999</v>
+      </c>
+      <c r="G8" s="11">
+        <v>330.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10">
+        <v>48</v>
+      </c>
+      <c r="E9" s="11">
+        <v>299.83600000000001</v>
+      </c>
+      <c r="F9" s="11">
+        <v>346.404</v>
+      </c>
+      <c r="G9" s="11">
+        <v>341.61700000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24.75" thickBot="1">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10">
+        <v>54</v>
+      </c>
+      <c r="E10" s="11">
+        <v>366.94799999999998</v>
+      </c>
+      <c r="F10" s="11">
+        <v>374.13600000000002</v>
+      </c>
+      <c r="G10" s="11">
+        <v>355.37599999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="D11" s="10">
+        <v>60</v>
+      </c>
+      <c r="E11" s="11">
+        <v>371.791</v>
+      </c>
+      <c r="F11" s="11">
+        <v>350.18900000000002</v>
+      </c>
+      <c r="G11" s="11">
+        <v>302.77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="D12" s="10">
+        <v>120</v>
+      </c>
+      <c r="E12" s="11">
+        <v>544.399</v>
+      </c>
+      <c r="F12" s="11">
+        <v>503.33800000000002</v>
+      </c>
+      <c r="G12" s="11">
+        <v>432.06400000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1">
+      <c r="D13" s="10">
+        <v>180</v>
+      </c>
+      <c r="E13" s="11">
+        <v>788.77800000000002</v>
+      </c>
+      <c r="F13" s="11">
+        <v>624.38400000000001</v>
+      </c>
+      <c r="G13" s="11">
+        <v>559.83699999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1">
+      <c r="D14" s="10">
+        <v>240</v>
+      </c>
+      <c r="E14" s="11">
+        <v>993.048</v>
+      </c>
+      <c r="F14" s="11">
+        <v>725.59699999999998</v>
+      </c>
+      <c r="G14" s="11">
+        <v>651.03099999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1">
+      <c r="D15" s="10">
+        <v>300</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1133.097</v>
+      </c>
+      <c r="F15" s="11">
+        <v>844.625</v>
+      </c>
+      <c r="G15" s="11">
+        <v>786.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1">
+      <c r="D16" s="10">
+        <v>360</v>
+      </c>
+      <c r="E16" s="11">
+        <v>1391.537</v>
+      </c>
+      <c r="F16" s="11">
+        <v>972.55799999999999</v>
+      </c>
+      <c r="G16" s="11">
+        <v>896.05</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="15" thickBot="1">
+      <c r="D17" s="10">
+        <v>420</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1564.385</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1111.2940000000001</v>
+      </c>
+      <c r="G17" s="11">
+        <v>959.03</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" ht="15" thickBot="1">
+      <c r="D18" s="10">
+        <v>480</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1739.7149999999999</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1315.67</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1068.357</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="15" thickBot="1">
+      <c r="D19" s="10">
+        <v>540</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1983.9169999999999</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1386.5940000000001</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1175.758</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="15" thickBot="1">
+      <c r="D20" s="10">
+        <v>600</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2242.5030000000002</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1524.6469999999999</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1271.675</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>